<commit_message>
use new seprate str instead of \t; support excel ommit field
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/ConfigData.xlsx
+++ b/ExcelTool/bin/table/ConfigData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyGitHub\ExcelTool\ExcelTool\bin\table\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1968A3F-636E-4604-AB87-8E2B95844B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConfigData" sheetId="6" r:id="rId1"/>
@@ -96,6 +102,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>1.</t>
@@ -105,6 +112,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -125,6 +133,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>4</t>
@@ -134,6 +143,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -154,6 +164,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -163,6 +174,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>.3</t>
@@ -177,6 +189,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>0</t>
@@ -186,6 +199,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>.5</t>
@@ -311,6 +325,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>G</t>
@@ -320,6 +335,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>ame02，推的目标的角色ID</t>
@@ -331,6 +347,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>2</t>
@@ -340,6 +357,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>0000</t>
@@ -351,6 +369,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>Game</t>
@@ -360,6 +379,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>02，蓝色方玩家角色列表</t>
@@ -383,6 +403,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>3</t>
@@ -392,6 +413,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>00</t>
@@ -421,6 +443,7 @@
         <sz val="11"/>
         <color rgb="FFC00000"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>1,1</t>
@@ -430,6 +453,7 @@
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>,2,5</t>
@@ -439,6 +463,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>,</t>
@@ -448,6 +473,7 @@
         <sz val="11"/>
         <color theme="8" tint="-0.249977111117893"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>-2,-5</t>
@@ -457,6 +483,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
         <charset val="134"/>
       </rPr>
       <t>,2,0</t>
@@ -505,15 +532,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,11 +548,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -537,6 +562,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -544,164 +570,39 @@
       <sz val="11"/>
       <color theme="2" tint="-0.499984740745262"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="8" tint="-0.249977111117893"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -722,204 +623,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599963377788629"/>
+        <fgColor theme="5" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599963377788629"/>
+        <fgColor theme="7" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599963377788629"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -955,251 +676,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1219,31 +701,31 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1261,13 +743,13 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1325,56 +807,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="百分比" xfId="3" builtinId="5"/>
-    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8"/>
-    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
-    <cellStyle name="注释" xfId="8" builtinId="10"/>
-    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
-    <cellStyle name="标题" xfId="10" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
-    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="输入" xfId="16" builtinId="20"/>
-    <cellStyle name="输出" xfId="17" builtinId="21"/>
-    <cellStyle name="计算" xfId="18" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
-    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="好" xfId="22" builtinId="26"/>
-    <cellStyle name="差" xfId="23" builtinId="27"/>
-    <cellStyle name="适中" xfId="24" builtinId="28"/>
-    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
-    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
-    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1392,6 +827,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1649,19 +1087,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2"/>
     <col min="2" max="2" width="110.625" style="3" customWidth="1"/>
@@ -1670,7 +1108,7 @@
     <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +1119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1692,12 +1130,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
@@ -1708,18 +1146,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="12">
         <v>1</v>
       </c>
@@ -1730,7 +1168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:3">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="12">
         <v>2</v>
       </c>
@@ -1741,7 +1179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:3">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1752,7 +1190,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="15">
         <v>5</v>
       </c>
@@ -1763,7 +1201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="15">
         <v>6</v>
       </c>
@@ -1774,7 +1212,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="15">
         <v>8</v>
       </c>
@@ -1785,7 +1223,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="15">
         <v>9</v>
       </c>
@@ -1796,7 +1234,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -1807,18 +1245,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="15">
         <v>20</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" s="18"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="15">
         <v>25</v>
       </c>
@@ -1829,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="15">
         <v>201</v>
       </c>
@@ -1840,7 +1276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="15">
         <v>202</v>
       </c>
@@ -1851,7 +1287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="15">
         <v>203</v>
       </c>
@@ -1862,7 +1298,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="15">
         <v>210</v>
       </c>
@@ -1873,7 +1309,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="15">
         <v>211</v>
       </c>
@@ -1884,7 +1320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="15">
         <v>212</v>
       </c>
@@ -1895,7 +1331,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="15">
         <v>1001</v>
       </c>
@@ -1906,7 +1342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="15">
         <v>1002</v>
       </c>
@@ -1917,7 +1353,7 @@
         <v>8088</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>1010</v>
       </c>
@@ -1928,7 +1364,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1" spans="1:3">
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A25" s="20">
         <v>1100</v>
       </c>
@@ -1939,7 +1375,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" s="1" customFormat="1" spans="1:3">
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A26" s="20">
         <v>1101</v>
       </c>
@@ -1950,7 +1386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" s="1" customFormat="1" spans="1:3">
+    <row r="27" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A27" s="20">
         <v>1102</v>
       </c>
@@ -1961,7 +1397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" s="1" customFormat="1" spans="1:3">
+    <row r="28" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A28" s="20">
         <v>1103</v>
       </c>
@@ -1972,7 +1408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" s="1" customFormat="1" spans="1:3">
+    <row r="29" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A29" s="20">
         <v>1104</v>
       </c>
@@ -1983,7 +1419,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>2000</v>
       </c>
@@ -1994,7 +1430,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>2001</v>
       </c>
@@ -2005,7 +1441,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>2010</v>
       </c>
@@ -2016,7 +1452,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="23">
         <v>10000</v>
       </c>
@@ -2027,7 +1463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" s="23">
         <v>10001</v>
       </c>
@@ -2038,7 +1474,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="23">
         <v>10002</v>
       </c>
@@ -2049,7 +1485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="23">
         <v>10003</v>
       </c>
@@ -2060,7 +1496,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="23">
         <v>10004</v>
       </c>
@@ -2071,7 +1507,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="23">
         <v>10005</v>
       </c>
@@ -2082,7 +1518,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="23">
         <v>10006</v>
       </c>
@@ -2093,7 +1529,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="23">
         <v>10007</v>
       </c>
@@ -2104,7 +1540,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="27">
         <v>10008</v>
       </c>
@@ -2115,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="27">
         <v>10009</v>
       </c>
@@ -2126,7 +1562,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="23">
         <v>10010</v>
       </c>
@@ -2137,7 +1573,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="23">
         <v>10011</v>
       </c>
@@ -2148,7 +1584,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="23">
         <v>10012</v>
       </c>
@@ -2159,7 +1595,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="30">
         <v>20000</v>
       </c>
@@ -2170,7 +1606,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="30">
         <v>20001</v>
       </c>
@@ -2181,7 +1617,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="30">
         <v>20002</v>
       </c>
@@ -2192,7 +1628,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="30">
         <v>20010</v>
       </c>
@@ -2203,7 +1639,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="30">
         <v>20011</v>
       </c>
@@ -2214,7 +1650,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="33">
         <v>30001</v>
       </c>
@@ -2225,7 +1661,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="36">
         <v>30002</v>
       </c>
@@ -2236,7 +1672,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="36">
         <v>30003</v>
       </c>
@@ -2247,7 +1683,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="36">
         <v>30004</v>
       </c>
@@ -2258,7 +1694,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="36">
         <v>30005</v>
       </c>
@@ -2269,7 +1705,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="36">
         <v>30006</v>
       </c>
@@ -2280,7 +1716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="36">
         <v>30007</v>
       </c>
@@ -2291,7 +1727,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>100000</v>
       </c>
@@ -2302,7 +1738,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="2">
         <v>100001</v>
       </c>
@@ -2313,7 +1749,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="2">
         <v>100002</v>
       </c>
@@ -2325,15 +1761,15 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A1:A4 A6:C8 B5 B1:C3">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C30" r:id="rId1" display="http://172.16.10.45:10000/login_dy_live"/>
-    <hyperlink ref="C31" r:id="rId2" display="http://47.108.161.219:10000/login_dy_live"/>
+    <hyperlink ref="C30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C31" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>